<commit_message>
updated diagrams and stats
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfree\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden_Freedman\PennTURBO\Drivetrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Measurements</t>
   </si>
   <si>
-    <t>1 minute 44 seconds</t>
-  </si>
-  <si>
     <t>30 minutes 39 seconds</t>
   </si>
   <si>
@@ -68,13 +65,70 @@
     <t>45 hours 37 minutes 23 seconds</t>
   </si>
   <si>
-    <t>12 minutes 23 seconds</t>
+    <t>Homo Sapiens Expansion</t>
+  </si>
+  <si>
+    <t>266 seconds</t>
+  </si>
+  <si>
+    <t>Encounter and Measurements Expansion</t>
+  </si>
+  <si>
+    <t>Diagnoses Expansion</t>
+  </si>
+  <si>
+    <t>Prescriptions Expansion</t>
+  </si>
+  <si>
+    <t>5147 seconds</t>
+  </si>
+  <si>
+    <t>617 seconds</t>
+  </si>
+  <si>
+    <t>4387 seconds</t>
+  </si>
+  <si>
+    <t>2 hours 53 minutes 59 seconds</t>
+  </si>
+  <si>
+    <t>1 minute 23 seconds</t>
+  </si>
+  <si>
+    <t>3 seconds</t>
+  </si>
+  <si>
+    <t>47 seconds</t>
+  </si>
+  <si>
+    <t>6 seconds</t>
+  </si>
+  <si>
+    <t>21 seconds</t>
+  </si>
+  <si>
+    <t>29 seconds</t>
+  </si>
+  <si>
+    <t>13 minutes 1 second</t>
+  </si>
+  <si>
+    <t>444 seconds</t>
+  </si>
+  <si>
+    <t>62 seconds</t>
+  </si>
+  <si>
+    <t>238 seconds</t>
+  </si>
+  <si>
+    <t>3779 seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,8 +160,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -390,69 +446,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1000</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="1">
         <v>917369</v>
       </c>
       <c r="E2" s="1">
-        <v>3593791</v>
+        <v>3593773</v>
       </c>
       <c r="F2" s="1">
         <v>36184</v>
@@ -466,16 +538,28 @@
       <c r="I2" s="1">
         <v>51163</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>10000</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D3" s="1">
         <v>9380085</v>
@@ -495,17 +579,35 @@
       <c r="I3" s="1">
         <v>507875</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>100000</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D4" s="1">
         <v>89808702</v>
       </c>
+      <c r="E4" s="1">
+        <v>350150937</v>
+      </c>
       <c r="F4" s="1">
         <v>3587004</v>
       </c>
@@ -518,17 +620,31 @@
       <c r="I4" s="1">
         <v>4917038</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>1000000</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1">
         <v>894416550</v>
       </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="1">
         <v>35786086</v>
       </c>
@@ -541,8 +657,15 @@
       <c r="I5" s="1">
         <v>48793260</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
triple count switched to bigint
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>3779 seconds</t>
+  </si>
+  <si>
+    <t>99201 seconds</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,9 @@
       <c r="J5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
     </row>

</xml_diff>

<commit_message>
diagnoses finished for one million performance test
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>99201 seconds</t>
+  </si>
+  <si>
+    <t>14479 seconds</t>
   </si>
 </sst>
 </file>
@@ -451,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +669,9 @@
       <c r="K5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="M5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
performance charts and final performance stats
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayden_Freedman\PennTURBO\Drivetrain\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hfree\Drivetrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8916"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -129,12 +129,84 @@
   </si>
   <si>
     <t>14479 seconds</t>
+  </si>
+  <si>
+    <t>34,035 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42 hours 15 minutes 25 seconds  </t>
+  </si>
+  <si>
+    <t>Carnival Export Time As Log</t>
+  </si>
+  <si>
+    <t>Drivetrain Instantiation Time As Log</t>
+  </si>
+  <si>
+    <t>Homo Sapiens Expansion As Log</t>
+  </si>
+  <si>
+    <t>".477"</t>
+  </si>
+  <si>
+    <t>"1.46"</t>
+  </si>
+  <si>
+    <t>"2.42"</t>
+  </si>
+  <si>
+    <t>HCM Expansion as Log</t>
+  </si>
+  <si>
+    <t>"1.67"</t>
+  </si>
+  <si>
+    <t>"2.65"</t>
+  </si>
+  <si>
+    <t>"3.71"</t>
+  </si>
+  <si>
+    <t>"5.00"</t>
+  </si>
+  <si>
+    <t>Diagnosis Expansion as Log</t>
+  </si>
+  <si>
+    <t>".78"</t>
+  </si>
+  <si>
+    <t>"1.79"</t>
+  </si>
+  <si>
+    <t>"2.79"</t>
+  </si>
+  <si>
+    <t>"4.16"</t>
+  </si>
+  <si>
+    <t>Prescription Expansion as Log</t>
+  </si>
+  <si>
+    <t>"1.32"</t>
+  </si>
+  <si>
+    <t>"2.38"</t>
+  </si>
+  <si>
+    <t>"3.64"</t>
+  </si>
+  <si>
+    <t>"4.53"</t>
+  </si>
+  <si>
+    <t>"3.58"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,227 +524,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="11" max="11" width="39.140625" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.109375" customWidth="1"/>
+    <col min="14" max="14" width="26.109375" customWidth="1"/>
+    <col min="15" max="15" width="17.44140625" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" customWidth="1"/>
+    <col min="18" max="18" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="S1" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1000</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2">
+        <v>2.39</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2">
+        <v>1.92</v>
+      </c>
+      <c r="F2" s="1">
         <v>917369</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>3593773</v>
       </c>
-      <c r="F2" s="1">
+      <c r="H2" s="1">
         <v>36184</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="1">
         <v>6727</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="1">
         <v>46252</v>
       </c>
-      <c r="I2" s="1">
+      <c r="K2" s="1">
         <v>51163</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="S2" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>10000</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3">
+        <v>3.26</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3">
+        <v>2.89</v>
+      </c>
+      <c r="F3" s="1">
         <v>9380085</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <v>36609719</v>
       </c>
-      <c r="F3" s="1">
+      <c r="H3" s="1">
         <v>372297</v>
       </c>
-      <c r="G3" s="1">
+      <c r="I3" s="1">
         <v>69484</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>482093</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>507875</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="O3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="Q3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>100000</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F4" s="1">
         <v>89808702</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>350150937</v>
       </c>
-      <c r="F4" s="1">
+      <c r="H4" s="1">
         <v>3587004</v>
       </c>
-      <c r="G4" s="1">
+      <c r="I4" s="1">
         <v>675998</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J4" s="1">
         <v>4516160</v>
       </c>
-      <c r="I4" s="1">
+      <c r="K4" s="1">
         <v>4917038</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="O4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1000000</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1">
+      <c r="C5">
+        <v>5.22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>5.18</v>
+      </c>
+      <c r="F5" s="1">
         <v>894416550</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
+        <v>3487368869</v>
+      </c>
+      <c r="H5" s="1">
         <v>35786086</v>
       </c>
-      <c r="G5" s="1">
+      <c r="I5" s="1">
         <v>6703298</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J5" s="1">
         <v>45073629</v>
       </c>
-      <c r="I5" s="1">
+      <c r="K5" s="1">
         <v>48793260</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="M5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="O5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="2"/>
+      <c r="Q5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added error message for missing repo
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -563,14 +563,15 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="4" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="29.21875" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" customWidth="1"/>
@@ -586,7 +587,10 @@
     <col min="17" max="17" width="20.5546875" customWidth="1"/>
     <col min="18" max="18" width="15.21875" customWidth="1"/>
     <col min="19" max="19" width="25.44140625" customWidth="1"/>
-    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="21" max="21" width="24.77734375" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" customWidth="1"/>
+    <col min="23" max="23" width="20.109375" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
some new tests and test making
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -62,9 +62,6 @@
     <t>3 hours 49 minutes 4 seconds</t>
   </si>
   <si>
-    <t>45 hours 37 minutes 23 seconds</t>
-  </si>
-  <si>
     <t>Homo Sapiens Expansion</t>
   </si>
   <si>
@@ -237,6 +234,12 @@
   </si>
   <si>
     <t>1 hour 32 minutes 45 seconds</t>
+  </si>
+  <si>
+    <t>45 hours 29 minutes 28 seconds</t>
+  </si>
+  <si>
+    <t>2937 seconds</t>
   </si>
 </sst>
 </file>
@@ -562,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -601,16 +604,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -631,40 +634,40 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.3">
@@ -678,10 +681,10 @@
         <v>2.39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2">
         <v>1.92</v>
@@ -705,28 +708,28 @@
         <v>51163</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
@@ -740,10 +743,10 @@
         <v>3.26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>2.89</v>
@@ -767,28 +770,28 @@
         <v>507875</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="T3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
@@ -802,10 +805,10 @@
         <v>4.1399999999999997</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4">
         <v>4.0199999999999996</v>
@@ -829,40 +832,40 @@
         <v>4917038</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="T4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
@@ -870,19 +873,19 @@
         <v>1000000</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C5">
         <v>5.22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5">
         <v>5.18</v>
       </c>
       <c r="G5" s="1">
-        <v>894416550</v>
+        <v>903373439</v>
       </c>
       <c r="H5" s="1">
         <v>3487368869</v>
@@ -900,28 +903,31 @@
         <v>48793260</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="T5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing snapshot test template and new tests
</commit_message>
<xml_diff>
--- a/Semantic_expander_time_stats.xlsx
+++ b/Semantic_expander_time_stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Patient Cohort Size</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>2937 seconds</t>
+  </si>
+  <si>
+    <t>20 hours 33 minutes</t>
   </si>
 </sst>
 </file>
@@ -565,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,6 +884,9 @@
       <c r="D5" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
       <c r="F5">
         <v>5.18</v>
       </c>
@@ -888,7 +894,7 @@
         <v>903373439</v>
       </c>
       <c r="H5" s="1">
-        <v>3487368869</v>
+        <v>3522298786</v>
       </c>
       <c r="I5" s="1">
         <v>35786086</v>

</xml_diff>